<commit_message>
Merging prediction and classification into a single repo
</commit_message>
<xml_diff>
--- a/Classification Results/Augmented Data/Full VPOP Classification/By Diagnosis/Control 0 (30, 11, 3, 38, 29)/MDD 0 (41, 8, 15, 16, 33)/ANN_128nodes_Uniform0.05Virtual_Control(30, 11, 3, 38, 29)_MDD(41, 8, 15, 16, 33)_100perPatient_batchsize10_20maxITER_StandardizeAll_smoothing0_dropout0.5.xlsx
+++ b/Classification Results/Augmented Data/Full VPOP Classification/By Diagnosis/Control 0 (30, 11, 3, 38, 29)/MDD 0 (41, 8, 15, 16, 33)/ANN_128nodes_Uniform0.05Virtual_Control(30, 11, 3, 38, 29)_MDD(41, 8, 15, 16, 33)_100perPatient_batchsize10_20maxITER_StandardizeAll_smoothing0_dropout0.5.xlsx
@@ -456,10 +456,10 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.9778142814062644</v>
+        <v>0.9999998079147523</v>
       </c>
       <c r="E2">
-        <v>0.9778142814062644</v>
+        <v>0.9999998079147523</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -470,10 +470,10 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0.9999999999909195</v>
+        <v>0.9999999977843042</v>
       </c>
       <c r="E3">
-        <v>0.9999999999909195</v>
+        <v>0.9999999977843042</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -484,10 +484,10 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>9.256073547630016E-20</v>
+        <v>1.236224896776247E-27</v>
       </c>
       <c r="E4">
-        <v>9.256073547630016E-20</v>
+        <v>1.236224896776247E-27</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -498,10 +498,10 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0.9967614897338082</v>
+        <v>0.9901112600426142</v>
       </c>
       <c r="E5">
-        <v>0.9967614897338082</v>
+        <v>0.9901112600426142</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -512,10 +512,10 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>0.9999968729170366</v>
+        <v>0.9999919240617908</v>
       </c>
       <c r="E6">
-        <v>0.9999968729170366</v>
+        <v>0.9999919240617908</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -526,10 +526,10 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>5.565193715005374E-06</v>
+        <v>0.002131138354101981</v>
       </c>
       <c r="E7">
-        <v>0.999994434806285</v>
+        <v>0.9978688616458981</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -540,10 +540,10 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>0.9988336575337369</v>
+        <v>0.9999999999998541</v>
       </c>
       <c r="E8">
-        <v>0.001166342466263126</v>
+        <v>1.458833054357456E-13</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -551,13 +551,13 @@
         <v>13</v>
       </c>
       <c r="C9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>0.01466939004401452</v>
+        <v>0.9999999999964497</v>
       </c>
       <c r="E9">
-        <v>0.9853306099559854</v>
+        <v>3.550271188146326E-12</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -588,10 +588,10 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>6.39633846282959</v>
+        <v>5.788710594177246</v>
       </c>
       <c r="G11">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>